<commit_message>
supply additional data into trainning_asp
This is additional data of "Các topic có đồ án" which indicate topics in the Demo application wrote by ASP.NET CORE 3.1
</commit_message>
<xml_diff>
--- a/Report tình hình demo/PhanCongTask.xlsx
+++ b/Report tình hình demo/PhanCongTask.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CDW1 De Nop\CDW1-Reponsitory\Report tình hình demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Trainning_asp.net\training_asp\Report tình hình demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D58B08-5935-4CEF-97A1-15EB85081D2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F167DBC-C139-4AD9-A624-EE90189C1988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{8836B1C6-3DE2-4218-8326-5584A6B8BE86}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{8836B1C6-3DE2-4218-8326-5584A6B8BE86}"/>
   </bookViews>
   <sheets>
     <sheet name="Nguyễn Y Trinh" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="81">
   <si>
     <t>Task 19/10/2020</t>
   </si>
@@ -387,6 +387,9 @@
   </si>
   <si>
     <t>Công cụ phát triển demo</t>
+  </si>
+  <si>
+    <t>Dự kiến hết ngày 5/11/2020</t>
   </si>
 </sst>
 </file>
@@ -611,11 +614,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -629,8 +632,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -641,7 +650,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -649,12 +658,6 @@
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -981,7 +984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99125B8A-366B-403E-BCC2-11FEF48DDC0C}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
@@ -1036,7 +1039,7 @@
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
       <c r="F5" s="21"/>
-      <c r="G5" s="20">
+      <c r="G5" s="19">
         <v>0.65</v>
       </c>
       <c r="H5" s="18"/>
@@ -1055,7 +1058,7 @@
       <c r="I6" s="18"/>
     </row>
     <row r="7" spans="1:9" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="20" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="18"/>
@@ -1120,11 +1123,11 @@
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
       <c r="F13" s="21"/>
-      <c r="G13" s="20">
+      <c r="G13" s="19">
         <v>0.85</v>
       </c>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
     </row>
     <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B14" s="21" t="s">
@@ -1134,21 +1137,21 @@
       <c r="D14" s="21"/>
       <c r="E14" s="21"/>
       <c r="F14" s="21"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
     </row>
     <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="20" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
     </row>
     <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B16" s="21" t="s">
@@ -1158,9 +1161,9 @@
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
       <c r="F16" s="21"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
@@ -1208,11 +1211,11 @@
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
-      <c r="G22" s="20">
+      <c r="G22" s="19">
         <v>0.9</v>
       </c>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
     </row>
     <row r="23" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="22"/>
@@ -1220,9 +1223,9 @@
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
     </row>
     <row r="24" spans="1:9" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="22"/>
@@ -1230,9 +1233,9 @@
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
     </row>
     <row r="25" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="21"/>
@@ -1240,9 +1243,9 @@
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
       <c r="F25" s="21"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
@@ -1283,48 +1286,48 @@
       <c r="I30" s="18"/>
     </row>
     <row r="31" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="19" t="s">
+      <c r="B31" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="20">
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="19">
         <v>0.9</v>
       </c>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
     </row>
     <row r="32" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
     </row>
     <row r="33" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
     </row>
     <row r="34" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="15" t="s">
@@ -1365,48 +1368,48 @@
       <c r="I40" s="18"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="20">
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="19">
         <v>0.9</v>
       </c>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B42" s="19"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B43" s="19"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
     </row>
     <row r="44" spans="1:9" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="19"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="15" t="s">
@@ -1447,56 +1450,71 @@
       <c r="I50" s="18"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B51" s="19" t="s">
+      <c r="B51" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="20">
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="19">
         <v>1</v>
       </c>
-      <c r="H51" s="20"/>
-      <c r="I51" s="20"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B52" s="19"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="20"/>
-      <c r="H52" s="20"/>
-      <c r="I52" s="20"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B53" s="19"/>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="20"/>
-      <c r="H53" s="20"/>
-      <c r="I53" s="20"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="19"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B54" s="19"/>
-      <c r="C54" s="19"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="19"/>
-      <c r="F54" s="19"/>
-      <c r="G54" s="20"/>
-      <c r="H54" s="20"/>
-      <c r="I54" s="20"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A27:D28"/>
-    <mergeCell ref="B29:F30"/>
-    <mergeCell ref="G29:I30"/>
-    <mergeCell ref="G31:I34"/>
-    <mergeCell ref="B31:F34"/>
+    <mergeCell ref="A47:D48"/>
+    <mergeCell ref="B49:F50"/>
+    <mergeCell ref="G49:I50"/>
+    <mergeCell ref="B51:F54"/>
+    <mergeCell ref="G51:I54"/>
+    <mergeCell ref="A37:D38"/>
+    <mergeCell ref="B39:F40"/>
+    <mergeCell ref="G39:I40"/>
+    <mergeCell ref="B41:F44"/>
+    <mergeCell ref="G41:I44"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="B3:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="G3:I4"/>
+    <mergeCell ref="G5:I7"/>
+    <mergeCell ref="A9:D10"/>
+    <mergeCell ref="B11:F12"/>
+    <mergeCell ref="G11:I12"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="G22:I25"/>
@@ -1508,26 +1526,11 @@
     <mergeCell ref="G20:I21"/>
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="B22:F24"/>
-    <mergeCell ref="G3:I4"/>
-    <mergeCell ref="G5:I7"/>
-    <mergeCell ref="A9:D10"/>
-    <mergeCell ref="B11:F12"/>
-    <mergeCell ref="G11:I12"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="B3:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="A37:D38"/>
-    <mergeCell ref="B39:F40"/>
-    <mergeCell ref="G39:I40"/>
-    <mergeCell ref="B41:F44"/>
-    <mergeCell ref="G41:I44"/>
-    <mergeCell ref="A47:D48"/>
-    <mergeCell ref="B49:F50"/>
-    <mergeCell ref="G49:I50"/>
-    <mergeCell ref="B51:F54"/>
-    <mergeCell ref="G51:I54"/>
+    <mergeCell ref="A27:D28"/>
+    <mergeCell ref="B29:F30"/>
+    <mergeCell ref="G29:I30"/>
+    <mergeCell ref="G31:I34"/>
+    <mergeCell ref="B31:F34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1593,7 +1596,7 @@
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
       <c r="F5" s="21"/>
-      <c r="G5" s="20">
+      <c r="G5" s="19">
         <v>0.75</v>
       </c>
       <c r="H5" s="18"/>
@@ -1612,7 +1615,7 @@
       <c r="I6" s="18"/>
     </row>
     <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="20" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="18"/>
@@ -1677,11 +1680,11 @@
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
       <c r="F13" s="21"/>
-      <c r="G13" s="20">
+      <c r="G13" s="19">
         <v>0.85</v>
       </c>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
     </row>
     <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B14" s="21" t="s">
@@ -1691,21 +1694,21 @@
       <c r="D14" s="21"/>
       <c r="E14" s="21"/>
       <c r="F14" s="21"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
     </row>
     <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="20" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
     </row>
     <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B16" s="21" t="s">
@@ -1715,9 +1718,9 @@
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
       <c r="F16" s="21"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
@@ -1765,11 +1768,11 @@
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
-      <c r="G22" s="20">
+      <c r="G22" s="19">
         <v>0.9</v>
       </c>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
     </row>
     <row r="23" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="22"/>
@@ -1777,9 +1780,9 @@
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
     </row>
     <row r="24" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="22"/>
@@ -1787,9 +1790,9 @@
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
     </row>
     <row r="25" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="22"/>
@@ -1797,9 +1800,9 @@
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
     </row>
     <row r="26" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="22"/>
@@ -1854,11 +1857,11 @@
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
-      <c r="G32" s="20">
+      <c r="G32" s="19">
         <v>0.9</v>
       </c>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B33" s="22"/>
@@ -1866,9 +1869,9 @@
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
       <c r="F33" s="22"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B34" s="22"/>
@@ -1876,9 +1879,9 @@
       <c r="D34" s="22"/>
       <c r="E34" s="22"/>
       <c r="F34" s="22"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
     </row>
     <row r="35" spans="1:9" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="22"/>
@@ -1886,9 +1889,9 @@
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
       <c r="F35" s="22"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-      <c r="I35" s="20"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="15" t="s">
@@ -1936,11 +1939,11 @@
       <c r="D41" s="22"/>
       <c r="E41" s="22"/>
       <c r="F41" s="22"/>
-      <c r="G41" s="20">
+      <c r="G41" s="19">
         <v>0.9</v>
       </c>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B42" s="22"/>
@@ -1948,9 +1951,9 @@
       <c r="D42" s="22"/>
       <c r="E42" s="22"/>
       <c r="F42" s="22"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B43" s="22"/>
@@ -1958,9 +1961,9 @@
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
       <c r="F43" s="22"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
     </row>
     <row r="44" spans="1:9" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="22"/>
@@ -1968,9 +1971,9 @@
       <c r="D44" s="22"/>
       <c r="E44" s="22"/>
       <c r="F44" s="22"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="15" t="s">
@@ -2011,63 +2014,61 @@
       <c r="I51" s="18"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B52" s="19" t="s">
+      <c r="B52" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="20">
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="19">
         <v>1</v>
       </c>
-      <c r="H52" s="20"/>
-      <c r="I52" s="20"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B53" s="19"/>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="20"/>
-      <c r="H53" s="20"/>
-      <c r="I53" s="20"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="19"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B54" s="19"/>
-      <c r="C54" s="19"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="19"/>
-      <c r="F54" s="19"/>
-      <c r="G54" s="20"/>
-      <c r="H54" s="20"/>
-      <c r="I54" s="20"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="19"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B55" s="19"/>
-      <c r="C55" s="19"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="19"/>
-      <c r="G55" s="20"/>
-      <c r="H55" s="20"/>
-      <c r="I55" s="20"/>
+      <c r="B55" s="20"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A28:D29"/>
-    <mergeCell ref="B30:F31"/>
-    <mergeCell ref="G30:I31"/>
-    <mergeCell ref="B32:F35"/>
-    <mergeCell ref="G32:I35"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="B3:F4"/>
-    <mergeCell ref="G3:I4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="G5:I7"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="A48:D49"/>
+    <mergeCell ref="B50:F51"/>
+    <mergeCell ref="G50:I51"/>
+    <mergeCell ref="B52:F55"/>
+    <mergeCell ref="G52:I55"/>
+    <mergeCell ref="A37:D38"/>
+    <mergeCell ref="B39:F40"/>
+    <mergeCell ref="G39:I40"/>
+    <mergeCell ref="B41:F44"/>
+    <mergeCell ref="G41:I44"/>
     <mergeCell ref="G22:I25"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="G13:I16"/>
@@ -2081,16 +2082,18 @@
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="A18:D19"/>
     <mergeCell ref="B20:F21"/>
-    <mergeCell ref="A37:D38"/>
-    <mergeCell ref="B39:F40"/>
-    <mergeCell ref="G39:I40"/>
-    <mergeCell ref="B41:F44"/>
-    <mergeCell ref="G41:I44"/>
-    <mergeCell ref="A48:D49"/>
-    <mergeCell ref="B50:F51"/>
-    <mergeCell ref="G50:I51"/>
-    <mergeCell ref="B52:F55"/>
-    <mergeCell ref="G52:I55"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="B3:F4"/>
+    <mergeCell ref="G3:I4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="G5:I7"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="A28:D29"/>
+    <mergeCell ref="B30:F31"/>
+    <mergeCell ref="G30:I31"/>
+    <mergeCell ref="B32:F35"/>
+    <mergeCell ref="G32:I35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2152,7 +2155,7 @@
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
       <c r="F5" s="21"/>
-      <c r="G5" s="20">
+      <c r="G5" s="19">
         <v>0.75</v>
       </c>
       <c r="H5" s="18"/>
@@ -2171,7 +2174,7 @@
       <c r="I6" s="18"/>
     </row>
     <row r="7" spans="1:9" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="20" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="18"/>
@@ -2236,11 +2239,11 @@
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
       <c r="F13" s="21"/>
-      <c r="G13" s="20">
+      <c r="G13" s="19">
         <v>0.85</v>
       </c>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
     </row>
     <row r="14" spans="1:9" ht="43.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="23" t="s">
@@ -2250,21 +2253,21 @@
       <c r="D14" s="21"/>
       <c r="E14" s="21"/>
       <c r="F14" s="21"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
     </row>
     <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="20" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
     </row>
     <row r="16" spans="1:9" ht="49.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="23" t="s">
@@ -2274,9 +2277,9 @@
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
       <c r="F16" s="21"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
     </row>
     <row r="17" spans="1:9" ht="49.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="23" t="s">
@@ -2286,9 +2289,9 @@
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
       <c r="F17" s="23"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
@@ -2336,11 +2339,11 @@
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
-      <c r="G23" s="20">
+      <c r="G23" s="19">
         <v>0.9</v>
       </c>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
     </row>
     <row r="24" spans="1:9" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="22"/>
@@ -2348,9 +2351,9 @@
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
     </row>
     <row r="25" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="22"/>
@@ -2358,9 +2361,9 @@
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
     </row>
     <row r="26" spans="1:9" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="22"/>
@@ -2368,9 +2371,9 @@
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B27" s="24"/>
@@ -2425,11 +2428,11 @@
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
-      <c r="G32" s="20">
+      <c r="G32" s="19">
         <v>0.9</v>
       </c>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B33" s="22"/>
@@ -2437,9 +2440,9 @@
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
       <c r="F33" s="22"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B34" s="22"/>
@@ -2447,9 +2450,9 @@
       <c r="D34" s="22"/>
       <c r="E34" s="22"/>
       <c r="F34" s="22"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B35" s="22"/>
@@ -2457,9 +2460,9 @@
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
       <c r="F35" s="22"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-      <c r="I35" s="20"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="15" t="s">
@@ -2507,11 +2510,11 @@
       <c r="D41" s="22"/>
       <c r="E41" s="22"/>
       <c r="F41" s="22"/>
-      <c r="G41" s="20">
+      <c r="G41" s="19">
         <v>0.85</v>
       </c>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B42" s="22"/>
@@ -2519,9 +2522,9 @@
       <c r="D42" s="22"/>
       <c r="E42" s="22"/>
       <c r="F42" s="22"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B43" s="22"/>
@@ -2529,9 +2532,9 @@
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
       <c r="F43" s="22"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
     </row>
     <row r="44" spans="1:9" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="22"/>
@@ -2539,9 +2542,9 @@
       <c r="D44" s="22"/>
       <c r="E44" s="22"/>
       <c r="F44" s="22"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="15" t="s">
@@ -2582,56 +2585,73 @@
       <c r="I50" s="18"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B51" s="19" t="s">
+      <c r="B51" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="20">
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="19">
         <v>1</v>
       </c>
-      <c r="H51" s="20"/>
-      <c r="I51" s="20"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B52" s="19"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="20"/>
-      <c r="H52" s="20"/>
-      <c r="I52" s="20"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B53" s="19"/>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="20"/>
-      <c r="H53" s="20"/>
-      <c r="I53" s="20"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="19"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B54" s="19"/>
-      <c r="C54" s="19"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="19"/>
-      <c r="F54" s="19"/>
-      <c r="G54" s="20"/>
-      <c r="H54" s="20"/>
-      <c r="I54" s="20"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A28:D29"/>
-    <mergeCell ref="B30:F31"/>
-    <mergeCell ref="G30:I31"/>
-    <mergeCell ref="B32:F35"/>
-    <mergeCell ref="G32:I35"/>
+    <mergeCell ref="A47:D48"/>
+    <mergeCell ref="B49:F50"/>
+    <mergeCell ref="G49:I50"/>
+    <mergeCell ref="B51:F54"/>
+    <mergeCell ref="G51:I54"/>
+    <mergeCell ref="A37:D38"/>
+    <mergeCell ref="B39:F40"/>
+    <mergeCell ref="G39:I40"/>
+    <mergeCell ref="B41:F44"/>
+    <mergeCell ref="G41:I44"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="B3:F4"/>
+    <mergeCell ref="G3:I4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="G5:I7"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="A9:D10"/>
+    <mergeCell ref="B11:F12"/>
+    <mergeCell ref="G11:I12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="G13:I17"/>
     <mergeCell ref="B27:F27"/>
@@ -2642,28 +2662,11 @@
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="B23:F26"/>
-    <mergeCell ref="A9:D10"/>
-    <mergeCell ref="B11:F12"/>
-    <mergeCell ref="G11:I12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="B3:F4"/>
-    <mergeCell ref="G3:I4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="G5:I7"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="A37:D38"/>
-    <mergeCell ref="B39:F40"/>
-    <mergeCell ref="G39:I40"/>
-    <mergeCell ref="B41:F44"/>
-    <mergeCell ref="G41:I44"/>
-    <mergeCell ref="A47:D48"/>
-    <mergeCell ref="B49:F50"/>
-    <mergeCell ref="G49:I50"/>
-    <mergeCell ref="B51:F54"/>
-    <mergeCell ref="G51:I54"/>
+    <mergeCell ref="A28:D29"/>
+    <mergeCell ref="B30:F31"/>
+    <mergeCell ref="G30:I31"/>
+    <mergeCell ref="B32:F35"/>
+    <mergeCell ref="G32:I35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2673,8 +2676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B7E3A1-86AB-4E83-8004-6814428C79D0}">
   <dimension ref="A1:U59"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59:B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2687,21 +2690,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
       <c r="N1" s="9"/>
       <c r="O1" s="9"/>
       <c r="P1" s="9"/>
@@ -2712,19 +2715,19 @@
       <c r="U1" s="9"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
       <c r="N2" s="9"/>
       <c r="O2" s="9"/>
       <c r="P2" s="9"/>
@@ -2735,19 +2738,19 @@
       <c r="U2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
       <c r="N3" s="9"/>
       <c r="O3" s="9"/>
       <c r="P3" s="9"/>
@@ -2763,28 +2766,28 @@
       </c>
     </row>
     <row r="6" spans="1:21" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
     </row>
     <row r="7" spans="1:21" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
     </row>
     <row r="8" spans="1:21" ht="21" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
@@ -2792,10 +2795,10 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="26"/>
+      <c r="B9" s="28"/>
     </row>
     <row r="10" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
@@ -2821,10 +2824,10 @@
       <c r="C11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="28"/>
+      <c r="E11" s="30"/>
       <c r="F11" s="6">
         <v>0.65</v>
       </c>
@@ -2837,10 +2840,10 @@
       <c r="C12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="7">
         <v>0.75</v>
       </c>
@@ -2853,25 +2856,25 @@
       <c r="C13" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="D13" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="28"/>
+      <c r="E13" s="30"/>
       <c r="F13" s="6">
         <v>0.65</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="29"/>
+      <c r="B15" s="25"/>
     </row>
     <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="26"/>
+      <c r="B17" s="28"/>
     </row>
     <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
@@ -2897,10 +2900,10 @@
       <c r="C19" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="27" t="s">
+      <c r="D19" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="28"/>
+      <c r="E19" s="30"/>
       <c r="F19" s="6">
         <v>0.85</v>
       </c>
@@ -2913,10 +2916,10 @@
       <c r="C20" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="27" t="s">
+      <c r="D20" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="28"/>
+      <c r="E20" s="30"/>
       <c r="F20" s="7">
         <v>0.85</v>
       </c>
@@ -2929,25 +2932,25 @@
       <c r="C21" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="27" t="s">
+      <c r="D21" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="28"/>
+      <c r="E21" s="30"/>
       <c r="F21" s="6">
         <v>0.85</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="29"/>
+      <c r="B23" s="25"/>
     </row>
     <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="A25" s="26" t="s">
+      <c r="A25" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="26"/>
+      <c r="B25" s="28"/>
     </row>
     <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
@@ -2973,10 +2976,10 @@
       <c r="C27" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="27" t="s">
+      <c r="D27" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="E27" s="28"/>
+      <c r="E27" s="30"/>
       <c r="F27" s="6">
         <v>0.9</v>
       </c>
@@ -2989,10 +2992,10 @@
       <c r="C28" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="27" t="s">
+      <c r="D28" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="E28" s="28"/>
+      <c r="E28" s="30"/>
       <c r="F28" s="7">
         <v>0.9</v>
       </c>
@@ -3005,19 +3008,19 @@
       <c r="C29" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="27" t="s">
+      <c r="D29" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="E29" s="28"/>
+      <c r="E29" s="30"/>
       <c r="F29" s="6">
         <v>0.75</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="29"/>
+      <c r="B31" s="25"/>
     </row>
     <row r="33" spans="1:6" ht="21" x14ac:dyDescent="0.4">
       <c r="A33" s="3" t="s">
@@ -3025,10 +3028,10 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="A35" s="26" t="s">
+      <c r="A35" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="26"/>
+      <c r="B35" s="28"/>
     </row>
     <row r="36" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A36" s="4"/>
@@ -3054,10 +3057,10 @@
       <c r="C37" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D37" s="27" t="s">
+      <c r="D37" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E37" s="28"/>
+      <c r="E37" s="30"/>
       <c r="F37" s="6">
         <v>0.9</v>
       </c>
@@ -3070,10 +3073,10 @@
       <c r="C38" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D38" s="27" t="s">
+      <c r="D38" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="E38" s="28"/>
+      <c r="E38" s="30"/>
       <c r="F38" s="7">
         <v>0.9</v>
       </c>
@@ -3086,25 +3089,25 @@
       <c r="C39" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D39" s="27" t="s">
+      <c r="D39" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="E39" s="28"/>
+      <c r="E39" s="30"/>
       <c r="F39" s="6">
         <v>0.85</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A41" s="29" t="s">
+      <c r="A41" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="B41" s="29"/>
+      <c r="B41" s="25"/>
     </row>
     <row r="43" spans="1:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="A43" s="26" t="s">
+      <c r="A43" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="B43" s="26"/>
+      <c r="B43" s="28"/>
     </row>
     <row r="44" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A44" s="4"/>
@@ -3130,10 +3133,10 @@
       <c r="C45" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D45" s="27" t="s">
+      <c r="D45" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="E45" s="28"/>
+      <c r="E45" s="30"/>
       <c r="F45" s="6">
         <v>0.9</v>
       </c>
@@ -3146,10 +3149,10 @@
       <c r="C46" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D46" s="27" t="s">
+      <c r="D46" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="E46" s="28"/>
+      <c r="E46" s="30"/>
       <c r="F46" s="7">
         <v>0.9</v>
       </c>
@@ -3162,19 +3165,19 @@
       <c r="C47" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D47" s="27" t="s">
+      <c r="D47" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="E47" s="28"/>
+      <c r="E47" s="30"/>
       <c r="F47" s="6">
         <v>0.85</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A49" s="29" t="s">
+      <c r="A49" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="B49" s="29"/>
+      <c r="B49" s="25"/>
     </row>
     <row r="51" spans="1:6" ht="21" x14ac:dyDescent="0.4">
       <c r="A51" s="3" t="s">
@@ -3182,10 +3185,10 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="A53" s="26" t="s">
+      <c r="A53" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="B53" s="26"/>
+      <c r="B53" s="28"/>
     </row>
     <row r="54" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A54" s="4"/>
@@ -3211,10 +3214,10 @@
       <c r="C55" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D55" s="32" t="s">
+      <c r="D55" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="E55" s="33"/>
+      <c r="E55" s="27"/>
       <c r="F55" s="6">
         <v>1</v>
       </c>
@@ -3227,10 +3230,10 @@
       <c r="C56" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D56" s="32" t="s">
+      <c r="D56" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="E56" s="33"/>
+      <c r="E56" s="27"/>
       <c r="F56" s="7">
         <v>1</v>
       </c>
@@ -3243,35 +3246,31 @@
       <c r="C57" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D57" s="32" t="s">
+      <c r="D57" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="E57" s="33"/>
+      <c r="E57" s="27"/>
       <c r="F57" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A59" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="B59" s="29"/>
+      <c r="A59" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B59" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="A1:M3"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A6:I7"/>
     <mergeCell ref="D37:E37"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D20:E20"/>
@@ -3282,15 +3281,19 @@
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A1:M3"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A6:I7"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D57:E57"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3302,7 +3305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1791377-1C35-45B2-B465-93A22957D374}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -3400,10 +3403,10 @@
       <c r="D7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="F7" s="28"/>
+      <c r="F7" s="30"/>
       <c r="G7" s="14" t="s">
         <v>72</v>
       </c>
@@ -3417,10 +3420,10 @@
       <c r="D8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="28"/>
+      <c r="F8" s="30"/>
       <c r="G8" s="13" t="s">
         <v>72</v>
       </c>
@@ -3434,10 +3437,10 @@
       <c r="D9" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="F9" s="28"/>
+      <c r="F9" s="30"/>
       <c r="G9" s="6" t="s">
         <v>77</v>
       </c>

</xml_diff>

<commit_message>
Update the documents and task manager
</commit_message>
<xml_diff>
--- a/Report tình hình demo/PhanCongTask.xlsx
+++ b/Report tình hình demo/PhanCongTask.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Trainning_asp.net\training_asp\Report tình hình demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F167DBC-C139-4AD9-A624-EE90189C1988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15853211-21EC-4552-AF45-4D7C03243560}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{8836B1C6-3DE2-4218-8326-5584A6B8BE86}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="82">
   <si>
     <t>Task 19/10/2020</t>
   </si>
@@ -320,10 +320,6 @@
   </si>
   <si>
     <t>18211TT2467</t>
-  </si>
-  <si>
-    <t>Sass,html,bootrap4,javascript
-,jquery</t>
   </si>
   <si>
     <t>Làm giao diện form ListUser
@@ -361,7 +357,10 @@
    -Hướng dẫn tích hợp sass</t>
   </si>
   <si>
-    <t>C#, ASP.NET MVC</t>
+    <t>Công cụ phát triển demo</t>
+  </si>
+  <si>
+    <t>Dự kiến hết ngày 5/11/2020</t>
   </si>
   <si>
     <t xml:space="preserve">Làm  chức năng Login email
@@ -377,19 +376,22 @@
    +User có quyền sửa thông tin của user, logout
 Viết docs ASP.NET CORE
    -Hướng dẫn gửi mail MailKit
-   -Giới thiệu tổng quan về MSTP server
-   -Giới thiệu về API google
-   -Hướng dẫn thiết lập API google vào trong ASP
+   - Hướng dẫn tích hợp Api login with google
    -Giới thiệu về UserIdentity và User Manager
    -Giới thiệu về RoleIdentity và Role Ma
    -Giới thiệu về SigninManager
 </t>
   </si>
   <si>
-    <t>Công cụ phát triển demo</t>
-  </si>
-  <si>
-    <t>Dự kiến hết ngày 5/11/2020</t>
+    <t>Sass,html,bootrap4,javascript
+,jquery,ASP.NET CORE MVC</t>
+  </si>
+  <si>
+    <t>C#, ASP.NET MVC,linq,Identity 
+authentication library,API Google,mailkit</t>
+  </si>
+  <si>
+    <t>hoành thành</t>
   </si>
 </sst>
 </file>
@@ -513,7 +515,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -536,37 +538,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -587,9 +563,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -601,6 +574,9 @@
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -662,10 +638,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1541,7 +1520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15090D6B-08CD-4719-A84F-A67CB64E41D5}">
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="L55" sqref="L55"/>
     </sheetView>
   </sheetViews>
@@ -2676,8 +2655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B7E3A1-86AB-4E83-8004-6814428C79D0}">
   <dimension ref="A1:U59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59:B59"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3256,7 +3235,7 @@
     </row>
     <row r="59" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A59" s="25" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B59" s="25"/>
     </row>
@@ -3306,7 +3285,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3318,6 +3297,7 @@
     <col min="5" max="5" width="13.44140625" customWidth="1"/>
     <col min="6" max="6" width="33.109375" customWidth="1"/>
     <col min="7" max="7" width="35.33203125" customWidth="1"/>
+    <col min="8" max="8" width="23.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -3355,29 +3335,29 @@
       <c r="N2" s="34"/>
     </row>
     <row r="3" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
       <c r="C6" s="8" t="s">
         <v>70</v>
       </c>
@@ -3387,140 +3367,151 @@
       <c r="E6" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="35"/>
       <c r="G6" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="1:14" ht="276" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="30"/>
+      <c r="G7" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-    </row>
-    <row r="7" spans="1:14" ht="276" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="30"/>
-      <c r="G7" s="14" t="s">
+      <c r="H7" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="281.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="29" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" ht="281.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="10" t="s">
+      <c r="F8" s="30"/>
+      <c r="G8" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" s="30"/>
-      <c r="G8" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="14" t="s">
         <v>35</v>
       </c>
       <c r="E9" s="29" t="s">
         <v>78</v>
       </c>
       <c r="F9" s="30"/>
-      <c r="G9" s="6" t="s">
-        <v>77</v>
+      <c r="G9" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" s="37">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
     </row>
     <row r="12" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
     </row>
     <row r="14" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
     </row>
     <row r="17" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
     </row>
     <row r="18" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
     </row>
     <row r="20" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
     </row>
     <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>

</xml_diff>

<commit_message>
update task manager 2 times
</commit_message>
<xml_diff>
--- a/Report tình hình demo/PhanCongTask.xlsx
+++ b/Report tình hình demo/PhanCongTask.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Trainning_asp.net\training_asp\Report tình hình demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15853211-21EC-4552-AF45-4D7C03243560}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B32F6D-7675-470A-86F2-7F05FD375BC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{8836B1C6-3DE2-4218-8326-5584A6B8BE86}"/>
   </bookViews>
@@ -578,6 +578,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -590,11 +596,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -608,14 +614,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -626,7 +626,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -635,16 +635,16 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -973,80 +973,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="18" t="s">
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
     </row>
     <row r="4" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
     </row>
     <row r="5" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="19">
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="22">
         <v>0.65</v>
       </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
     </row>
     <row r="6" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
     </row>
     <row r="7" spans="1:9" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
     </row>
     <row r="8" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
@@ -1057,443 +1057,428 @@
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18" t="s">
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
     </row>
     <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="19">
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="22">
         <v>0.85</v>
       </c>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
     </row>
     <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
     </row>
     <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
     </row>
     <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="18" t="s">
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
     </row>
     <row r="22" spans="1:9" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="19">
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="22">
         <v>0.9</v>
       </c>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
     </row>
     <row r="23" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
     </row>
     <row r="24" spans="1:9" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
     </row>
     <row r="25" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="16"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="18" t="s">
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
     </row>
     <row r="31" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="19">
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="22">
         <v>0.9</v>
       </c>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
     </row>
     <row r="32" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
     </row>
     <row r="33" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
     </row>
     <row r="34" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="16"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="16"/>
-      <c r="B38" s="16"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="18" t="s">
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="19">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="22">
         <v>0.9</v>
       </c>
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="22"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="22"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="19"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
     </row>
     <row r="44" spans="1:9" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="19"/>
-      <c r="H44" s="19"/>
-      <c r="I44" s="19"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B47" s="16"/>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="16"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="16"/>
+      <c r="A48" s="18"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B49" s="17" t="s">
+      <c r="B49" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C49" s="17"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="17"/>
-      <c r="G49" s="18" t="s">
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H49" s="18"/>
-      <c r="I49" s="18"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="20"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B50" s="17"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="18"/>
-      <c r="H50" s="18"/>
-      <c r="I50" s="18"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B51" s="20" t="s">
+      <c r="B51" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="19">
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="22">
         <v>1</v>
       </c>
-      <c r="H51" s="19"/>
-      <c r="I51" s="19"/>
+      <c r="H51" s="22"/>
+      <c r="I51" s="22"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B52" s="20"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
-      <c r="G52" s="19"/>
-      <c r="H52" s="19"/>
-      <c r="I52" s="19"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="22"/>
+      <c r="H52" s="22"/>
+      <c r="I52" s="22"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B53" s="20"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
-      <c r="G53" s="19"/>
-      <c r="H53" s="19"/>
-      <c r="I53" s="19"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="22"/>
+      <c r="H53" s="22"/>
+      <c r="I53" s="22"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="20"/>
-      <c r="G54" s="19"/>
-      <c r="H54" s="19"/>
-      <c r="I54" s="19"/>
+      <c r="B54" s="21"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="22"/>
+      <c r="H54" s="22"/>
+      <c r="I54" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A47:D48"/>
-    <mergeCell ref="B49:F50"/>
-    <mergeCell ref="G49:I50"/>
-    <mergeCell ref="B51:F54"/>
-    <mergeCell ref="G51:I54"/>
-    <mergeCell ref="A37:D38"/>
-    <mergeCell ref="B39:F40"/>
-    <mergeCell ref="G39:I40"/>
-    <mergeCell ref="B41:F44"/>
-    <mergeCell ref="G41:I44"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="B3:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="G3:I4"/>
-    <mergeCell ref="G5:I7"/>
-    <mergeCell ref="A9:D10"/>
-    <mergeCell ref="B11:F12"/>
-    <mergeCell ref="G11:I12"/>
+    <mergeCell ref="A27:D28"/>
+    <mergeCell ref="B29:F30"/>
+    <mergeCell ref="G29:I30"/>
+    <mergeCell ref="G31:I34"/>
+    <mergeCell ref="B31:F34"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="G22:I25"/>
@@ -1505,11 +1490,26 @@
     <mergeCell ref="G20:I21"/>
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="B22:F24"/>
-    <mergeCell ref="A27:D28"/>
-    <mergeCell ref="B29:F30"/>
-    <mergeCell ref="G29:I30"/>
-    <mergeCell ref="G31:I34"/>
-    <mergeCell ref="B31:F34"/>
+    <mergeCell ref="G3:I4"/>
+    <mergeCell ref="G5:I7"/>
+    <mergeCell ref="A9:D10"/>
+    <mergeCell ref="B11:F12"/>
+    <mergeCell ref="G11:I12"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="B3:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="A37:D38"/>
+    <mergeCell ref="B39:F40"/>
+    <mergeCell ref="G39:I40"/>
+    <mergeCell ref="B41:F44"/>
+    <mergeCell ref="G41:I44"/>
+    <mergeCell ref="A47:D48"/>
+    <mergeCell ref="B49:F50"/>
+    <mergeCell ref="G49:I50"/>
+    <mergeCell ref="B51:F54"/>
+    <mergeCell ref="G51:I54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1530,80 +1530,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="18" t="s">
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
     </row>
     <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="19">
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="22">
         <v>0.75</v>
       </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
     </row>
     <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
     </row>
     <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
     </row>
     <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
@@ -1614,440 +1614,442 @@
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18" t="s">
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
     </row>
     <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="19">
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="22">
         <v>0.85</v>
       </c>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
     </row>
     <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
     </row>
     <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
     </row>
     <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="18" t="s">
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
     </row>
     <row r="22" spans="1:9" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="19">
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="22">
         <v>0.9</v>
       </c>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
     </row>
     <row r="23" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
     </row>
     <row r="24" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
     </row>
     <row r="25" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
     </row>
     <row r="26" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="18" t="s">
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="19">
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="22">
         <v>0.9</v>
       </c>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
     </row>
     <row r="35" spans="1:9" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="22"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="16"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="16"/>
-      <c r="B38" s="16"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="18" t="s">
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B41" s="22" t="s">
+      <c r="B41" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="19">
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="22">
         <v>0.9</v>
       </c>
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="22"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B42" s="22"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="22"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B43" s="22"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="19"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
     </row>
     <row r="44" spans="1:9" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="22"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="22"/>
-      <c r="G44" s="19"/>
-      <c r="H44" s="19"/>
-      <c r="I44" s="19"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="15" t="s">
+      <c r="A48" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B48" s="16"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="16"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="16"/>
-      <c r="B49" s="16"/>
-      <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
+      <c r="A49" s="18"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B50" s="17" t="s">
+      <c r="B50" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="18" t="s">
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H50" s="18"/>
-      <c r="I50" s="18"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B51" s="17"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="18"/>
-      <c r="H51" s="18"/>
-      <c r="I51" s="18"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="20"/>
+      <c r="I51" s="20"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B52" s="20" t="s">
+      <c r="B52" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
-      <c r="G52" s="19">
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="22">
         <v>1</v>
       </c>
-      <c r="H52" s="19"/>
-      <c r="I52" s="19"/>
+      <c r="H52" s="22"/>
+      <c r="I52" s="22"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B53" s="20"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
-      <c r="G53" s="19"/>
-      <c r="H53" s="19"/>
-      <c r="I53" s="19"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="22"/>
+      <c r="H53" s="22"/>
+      <c r="I53" s="22"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="20"/>
-      <c r="G54" s="19"/>
-      <c r="H54" s="19"/>
-      <c r="I54" s="19"/>
+      <c r="B54" s="21"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="22"/>
+      <c r="H54" s="22"/>
+      <c r="I54" s="22"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B55" s="20"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="20"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="20"/>
-      <c r="G55" s="19"/>
-      <c r="H55" s="19"/>
-      <c r="I55" s="19"/>
+      <c r="B55" s="21"/>
+      <c r="C55" s="21"/>
+      <c r="D55" s="21"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="21"/>
+      <c r="G55" s="22"/>
+      <c r="H55" s="22"/>
+      <c r="I55" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A48:D49"/>
-    <mergeCell ref="B50:F51"/>
-    <mergeCell ref="G50:I51"/>
-    <mergeCell ref="B52:F55"/>
-    <mergeCell ref="G52:I55"/>
-    <mergeCell ref="A37:D38"/>
-    <mergeCell ref="B39:F40"/>
-    <mergeCell ref="G39:I40"/>
-    <mergeCell ref="B41:F44"/>
-    <mergeCell ref="G41:I44"/>
+    <mergeCell ref="A28:D29"/>
+    <mergeCell ref="B30:F31"/>
+    <mergeCell ref="G30:I31"/>
+    <mergeCell ref="B32:F35"/>
+    <mergeCell ref="G32:I35"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="B3:F4"/>
+    <mergeCell ref="G3:I4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="G5:I7"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
     <mergeCell ref="G22:I25"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="G13:I16"/>
@@ -2061,18 +2063,16 @@
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="A18:D19"/>
     <mergeCell ref="B20:F21"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="B3:F4"/>
-    <mergeCell ref="G3:I4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="G5:I7"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="A28:D29"/>
-    <mergeCell ref="B30:F31"/>
-    <mergeCell ref="G30:I31"/>
-    <mergeCell ref="B32:F35"/>
-    <mergeCell ref="G32:I35"/>
+    <mergeCell ref="A37:D38"/>
+    <mergeCell ref="B39:F40"/>
+    <mergeCell ref="G39:I40"/>
+    <mergeCell ref="B41:F44"/>
+    <mergeCell ref="G41:I44"/>
+    <mergeCell ref="A48:D49"/>
+    <mergeCell ref="B50:F51"/>
+    <mergeCell ref="G50:I51"/>
+    <mergeCell ref="B52:F55"/>
+    <mergeCell ref="G52:I55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2089,80 +2089,80 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="18" t="s">
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
     </row>
     <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="19">
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="22">
         <v>0.75</v>
       </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
     </row>
     <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
     </row>
     <row r="7" spans="1:9" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
     </row>
     <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
@@ -2173,464 +2173,447 @@
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18" t="s">
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
     </row>
     <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="19">
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="22">
         <v>0.85</v>
       </c>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
     </row>
     <row r="14" spans="1:9" ht="43.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
     </row>
     <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
     </row>
     <row r="16" spans="1:9" ht="49.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
     </row>
     <row r="17" spans="1:9" ht="49.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="16"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18" t="s">
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
     </row>
     <row r="23" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="19">
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="22">
         <v>0.9</v>
       </c>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
     </row>
     <row r="24" spans="1:9" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
     </row>
     <row r="25" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
     </row>
     <row r="26" spans="1:9" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="18" t="s">
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="19">
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="22">
         <v>0.9</v>
       </c>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B35" s="22"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="16"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="16"/>
-      <c r="B38" s="16"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="18" t="s">
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B41" s="22" t="s">
+      <c r="B41" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="19">
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="22">
         <v>0.85</v>
       </c>
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="22"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B42" s="22"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="22"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B43" s="22"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="19"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
     </row>
     <row r="44" spans="1:9" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="22"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="22"/>
-      <c r="G44" s="19"/>
-      <c r="H44" s="19"/>
-      <c r="I44" s="19"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B47" s="16"/>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="16"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="16"/>
+      <c r="A48" s="18"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B49" s="17" t="s">
+      <c r="B49" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C49" s="17"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="17"/>
-      <c r="G49" s="18" t="s">
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H49" s="18"/>
-      <c r="I49" s="18"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="20"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B50" s="17"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="18"/>
-      <c r="H50" s="18"/>
-      <c r="I50" s="18"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B51" s="20" t="s">
+      <c r="B51" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="19">
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="22">
         <v>1</v>
       </c>
-      <c r="H51" s="19"/>
-      <c r="I51" s="19"/>
+      <c r="H51" s="22"/>
+      <c r="I51" s="22"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B52" s="20"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
-      <c r="G52" s="19"/>
-      <c r="H52" s="19"/>
-      <c r="I52" s="19"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="22"/>
+      <c r="H52" s="22"/>
+      <c r="I52" s="22"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B53" s="20"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
-      <c r="G53" s="19"/>
-      <c r="H53" s="19"/>
-      <c r="I53" s="19"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="22"/>
+      <c r="H53" s="22"/>
+      <c r="I53" s="22"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="20"/>
-      <c r="G54" s="19"/>
-      <c r="H54" s="19"/>
-      <c r="I54" s="19"/>
+      <c r="B54" s="21"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="22"/>
+      <c r="H54" s="22"/>
+      <c r="I54" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A47:D48"/>
-    <mergeCell ref="B49:F50"/>
-    <mergeCell ref="G49:I50"/>
-    <mergeCell ref="B51:F54"/>
-    <mergeCell ref="G51:I54"/>
-    <mergeCell ref="A37:D38"/>
-    <mergeCell ref="B39:F40"/>
-    <mergeCell ref="G39:I40"/>
-    <mergeCell ref="B41:F44"/>
-    <mergeCell ref="G41:I44"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="B3:F4"/>
-    <mergeCell ref="G3:I4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="G5:I7"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="A9:D10"/>
-    <mergeCell ref="B11:F12"/>
-    <mergeCell ref="G11:I12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="A28:D29"/>
+    <mergeCell ref="B30:F31"/>
+    <mergeCell ref="G30:I31"/>
+    <mergeCell ref="B32:F35"/>
+    <mergeCell ref="G32:I35"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="G13:I17"/>
     <mergeCell ref="B27:F27"/>
@@ -2641,11 +2624,28 @@
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="B23:F26"/>
-    <mergeCell ref="A28:D29"/>
-    <mergeCell ref="B30:F31"/>
-    <mergeCell ref="G30:I31"/>
-    <mergeCell ref="B32:F35"/>
-    <mergeCell ref="G32:I35"/>
+    <mergeCell ref="A9:D10"/>
+    <mergeCell ref="B11:F12"/>
+    <mergeCell ref="G11:I12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="B3:F4"/>
+    <mergeCell ref="G3:I4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="G5:I7"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="A37:D38"/>
+    <mergeCell ref="B39:F40"/>
+    <mergeCell ref="G39:I40"/>
+    <mergeCell ref="B41:F44"/>
+    <mergeCell ref="G41:I44"/>
+    <mergeCell ref="A47:D48"/>
+    <mergeCell ref="B49:F50"/>
+    <mergeCell ref="G49:I50"/>
+    <mergeCell ref="B51:F54"/>
+    <mergeCell ref="G51:I54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2655,8 +2655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B7E3A1-86AB-4E83-8004-6814428C79D0}">
   <dimension ref="A1:U59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2669,21 +2669,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
       <c r="N1" s="9"/>
       <c r="O1" s="9"/>
       <c r="P1" s="9"/>
@@ -2694,19 +2694,19 @@
       <c r="U1" s="9"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
       <c r="N2" s="9"/>
       <c r="O2" s="9"/>
       <c r="P2" s="9"/>
@@ -2717,19 +2717,19 @@
       <c r="U2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
       <c r="N3" s="9"/>
       <c r="O3" s="9"/>
       <c r="P3" s="9"/>
@@ -2844,10 +2844,10 @@
       </c>
     </row>
     <row r="15" spans="1:21" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="25"/>
+      <c r="B15" s="31"/>
     </row>
     <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="28" t="s">
@@ -2920,10 +2920,10 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="25"/>
+      <c r="B23" s="31"/>
     </row>
     <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A25" s="28" t="s">
@@ -2996,10 +2996,10 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="25"/>
+      <c r="B31" s="31"/>
     </row>
     <row r="33" spans="1:6" ht="21" x14ac:dyDescent="0.4">
       <c r="A33" s="3" t="s">
@@ -3077,10 +3077,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A41" s="25" t="s">
+      <c r="A41" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="B41" s="25"/>
+      <c r="B41" s="31"/>
     </row>
     <row r="43" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A43" s="28" t="s">
@@ -3153,10 +3153,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A49" s="25" t="s">
+      <c r="A49" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="B49" s="25"/>
+      <c r="B49" s="31"/>
     </row>
     <row r="51" spans="1:6" ht="21" x14ac:dyDescent="0.4">
       <c r="A51" s="3" t="s">
@@ -3193,10 +3193,10 @@
       <c r="C55" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D55" s="26" t="s">
+      <c r="D55" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="E55" s="27"/>
+      <c r="E55" s="35"/>
       <c r="F55" s="6">
         <v>1</v>
       </c>
@@ -3209,10 +3209,10 @@
       <c r="C56" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D56" s="26" t="s">
+      <c r="D56" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="E56" s="27"/>
+      <c r="E56" s="35"/>
       <c r="F56" s="7">
         <v>1</v>
       </c>
@@ -3225,31 +3225,35 @@
       <c r="C57" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D57" s="26" t="s">
+      <c r="D57" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="E57" s="27"/>
+      <c r="E57" s="35"/>
       <c r="F57" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A59" s="25" t="s">
+      <c r="A59" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="B59" s="25"/>
+      <c r="B59" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A1:M3"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A6:I7"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D37:E37"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D20:E20"/>
@@ -3260,19 +3264,15 @@
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="A1:M3"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A6:I7"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3301,38 +3301,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
     </row>
     <row r="3" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
@@ -3364,14 +3364,14 @@
       <c r="D6" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="F6" s="35"/>
+      <c r="F6" s="37"/>
       <c r="G6" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="H6" s="36" t="s">
+      <c r="H6" s="15" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="11"/>
@@ -3392,7 +3392,7 @@
       <c r="G7" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="H7" s="37">
+      <c r="H7" s="16">
         <v>1</v>
       </c>
     </row>
@@ -3412,7 +3412,7 @@
       <c r="G8" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="H8" s="37">
+      <c r="H8" s="16">
         <v>1</v>
       </c>
     </row>
@@ -3432,7 +3432,7 @@
       <c r="G9" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="H9" s="37">
+      <c r="H9" s="16">
         <v>1</v>
       </c>
     </row>

</xml_diff>